<commit_message>
INTERNSHIP MODULES LIST UPDATED
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_InternshipModules.xlsx
+++ b/Datasets/UCD_EngArch_InternshipModules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B8958DA-AF2C-4F73-AC34-FE9C5106ACAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E75679C-73BA-4DE7-AAF0-0C26B889016E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC9AD590-2CC5-48AF-964A-7720A0F9A852}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>ARCT40520</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>MEEN41050</t>
+  </si>
+  <si>
+    <t>ME MSE PWE (Long)</t>
+  </si>
+  <si>
+    <t>MEEN40760</t>
+  </si>
+  <si>
+    <t>Professional Work Placement</t>
+  </si>
+  <si>
+    <t>MEEN40930</t>
+  </si>
+  <si>
+    <t>BSEN40230</t>
   </si>
 </sst>
 </file>
@@ -564,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D99C57-D38A-46AA-A5F2-4C64527FA5C1}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,6 +997,48 @@
         <v>9</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>